<commit_message>
Added some of the remaining landmarks in both excel file and xml map
</commit_message>
<xml_diff>
--- a/Posicion_Balizas.xlsx
+++ b/Posicion_Balizas.xlsx
@@ -5,33 +5,22 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cacha\Documents\MASTER\2ºCurso\1 Cuatri\Guiado y Navegación\TRABAJO\GITHUB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerko\Desktop\Master\GNR\robotJardinero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7963FE05-B2EC-49E3-8C00-4F5A5C6ABB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EBD192-E4D1-481A-BF41-8B12640BD0E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9750" yWindow="-10095" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>Nombre de la Baliza</t>
   </si>
@@ -205,6 +194,24 @@
   </si>
   <si>
     <t>12.4</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>7.2</t>
   </si>
 </sst>
 </file>
@@ -581,7 +588,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,11 +894,11 @@
       <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -901,20 +908,48 @@
       <c r="A23" t="s">
         <v>49</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>50</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>51</v>
       </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -927,12 +962,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100681D9EA2EA53234693ABE7ED0B1BBD91" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="8e15ced9fe71cb93d40cbb5cf5d0a7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="86abb9a5-2e62-43fb-99c2-51636a65f06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68d70a80704eaf3487fe7b7230d6f4bd" ns2:_="">
     <xsd:import namespace="86abb9a5-2e62-43fb-99c2-51636a65f06a"/>
@@ -1088,6 +1117,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1098,15 +1133,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{293788E5-653A-4F40-98E2-B64D9809623A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866EB587-322E-48EC-BC4E-31E5733649E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1124,6 +1150,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{293788E5-653A-4F40-98E2-B64D9809623A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3C161EA-027E-46D5-86AA-D09C5BC1632E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added integration project and small modifications to LM positions
</commit_message>
<xml_diff>
--- a/Posicion_Balizas.xlsx
+++ b/Posicion_Balizas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerko\Desktop\Master\GNR\robotJardinero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EBD192-E4D1-481A-BF41-8B12640BD0E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA4EF6-09DA-469A-9022-6FE7FD5FE6D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9750" yWindow="-10095" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>Nombre de la Baliza</t>
   </si>
@@ -94,12 +94,6 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>13.5</t>
-  </si>
-  <si>
-    <t>26.5</t>
-  </si>
-  <si>
     <t>9.2</t>
   </si>
   <si>
@@ -212,6 +206,15 @@
   </si>
   <si>
     <t>7.2</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>13.4</t>
+  </si>
+  <si>
+    <t>26.4</t>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,11 +631,11 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>23</v>
@@ -642,11 +645,11 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>23</v>
@@ -657,10 +660,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
@@ -671,10 +674,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
@@ -685,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>23</v>
@@ -699,10 +702,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -713,7 +716,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -727,10 +730,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
@@ -741,10 +744,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>23</v>
@@ -755,10 +758,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
@@ -769,10 +772,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
@@ -783,10 +786,10 @@
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>23</v>
@@ -797,10 +800,10 @@
         <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
@@ -814,7 +817,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
@@ -825,10 +828,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
@@ -839,10 +842,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>23</v>
@@ -850,13 +853,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>23</v>
@@ -864,13 +867,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>23</v>
@@ -878,13 +881,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
@@ -892,13 +895,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -906,13 +909,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -920,13 +923,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>23</v>
@@ -934,7 +937,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -944,7 +947,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -962,6 +965,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100681D9EA2EA53234693ABE7ED0B1BBD91" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="8e15ced9fe71cb93d40cbb5cf5d0a7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="86abb9a5-2e62-43fb-99c2-51636a65f06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68d70a80704eaf3487fe7b7230d6f4bd" ns2:_="">
     <xsd:import namespace="86abb9a5-2e62-43fb-99c2-51636a65f06a"/>
@@ -1117,12 +1126,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1133,6 +1136,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{293788E5-653A-4F40-98E2-B64D9809623A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866EB587-322E-48EC-BC4E-31E5733649E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1150,15 +1162,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{293788E5-653A-4F40-98E2-B64D9809623A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3C161EA-027E-46D5-86AA-D09C5BC1632E}">
   <ds:schemaRefs>

</xml_diff>